<commit_message>
add items to deduplication list
</commit_message>
<xml_diff>
--- a/ema_ingest/ema_exclusions.xlsx
+++ b/ema_ingest/ema_exclusions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdeluca/Research/Postdoc/ARPA-H/DrugList_V2/ema_ingest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdeluca/Research/Postdoc/ARPA-H/Matrix_repos/matrix-drug-list/ema_ingest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFD8FA9-84DC-A546-8C8A-0F811E2FA938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA94F965-30BD-1E46-A639-8F8C8F1B5882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FFA07BB0-444D-4F46-B712-47EE897B7BCD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>TECHNETIUM (99MTC) NOFETUMOMAB MERPENTAN</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <dimension ref="A1:A135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,7 +629,9 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>

</xml_diff>